<commit_message>
Carga ajustes eje x
</commit_message>
<xml_diff>
--- a/Datos/Rankings.xlsx
+++ b/Datos/Rankings.xlsx
@@ -92,16 +92,16 @@
     <t>USapiens</t>
   </si>
   <si>
-    <t>Bogotá</t>
+    <t>USAPIENS</t>
   </si>
   <si>
-    <t>Medellín</t>
+    <t>Puesto Bogotá</t>
   </si>
   <si>
-    <t>Palmira</t>
+    <t>Puesto Medellín</t>
   </si>
   <si>
-    <t>USAPIENS</t>
+    <t>Puesto Palmira</t>
   </si>
 </sst>
 </file>
@@ -452,14 +452,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95:B154"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I149" sqref="I149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -2347,7 +2347,7 @@
         <v>21</v>
       </c>
       <c r="B95" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C95">
         <v>2011</v>
@@ -2356,7 +2356,7 @@
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F95" s="2">
         <v>1</v>
@@ -2367,7 +2367,7 @@
         <v>21</v>
       </c>
       <c r="B96" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C96">
         <v>2011</v>
@@ -2376,7 +2376,7 @@
         <v>2</v>
       </c>
       <c r="E96" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F96" s="2">
         <v>1</v>
@@ -2387,7 +2387,7 @@
         <v>21</v>
       </c>
       <c r="B97" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C97">
         <v>2012</v>
@@ -2396,7 +2396,7 @@
         <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F97" s="2">
         <v>1</v>
@@ -2407,7 +2407,7 @@
         <v>21</v>
       </c>
       <c r="B98" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C98">
         <v>2012</v>
@@ -2416,7 +2416,7 @@
         <v>2</v>
       </c>
       <c r="E98" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F98" s="2">
         <v>1</v>
@@ -2427,7 +2427,7 @@
         <v>21</v>
       </c>
       <c r="B99" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C99">
         <v>2013</v>
@@ -2436,7 +2436,7 @@
         <v>1</v>
       </c>
       <c r="E99" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F99" s="2">
         <v>1</v>
@@ -2447,7 +2447,7 @@
         <v>21</v>
       </c>
       <c r="B100" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C100">
         <v>2013</v>
@@ -2456,7 +2456,7 @@
         <v>2</v>
       </c>
       <c r="E100" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F100" s="2">
         <v>1</v>
@@ -2467,7 +2467,7 @@
         <v>21</v>
       </c>
       <c r="B101" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C101">
         <v>2014</v>
@@ -2476,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="E101" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F101" s="2">
         <v>1</v>
@@ -2487,7 +2487,7 @@
         <v>21</v>
       </c>
       <c r="B102" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C102">
         <v>2014</v>
@@ -2496,7 +2496,7 @@
         <v>2</v>
       </c>
       <c r="E102" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F102" s="2">
         <v>1</v>
@@ -2507,7 +2507,7 @@
         <v>21</v>
       </c>
       <c r="B103" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C103">
         <v>2015</v>
@@ -2516,7 +2516,7 @@
         <v>1</v>
       </c>
       <c r="E103" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F103" s="2">
         <v>1</v>
@@ -2527,7 +2527,7 @@
         <v>21</v>
       </c>
       <c r="B104" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C104">
         <v>2015</v>
@@ -2536,7 +2536,7 @@
         <v>2</v>
       </c>
       <c r="E104" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F104" s="2">
         <v>1</v>
@@ -2547,7 +2547,7 @@
         <v>21</v>
       </c>
       <c r="B105" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C105">
         <v>2016</v>
@@ -2556,7 +2556,7 @@
         <v>1</v>
       </c>
       <c r="E105" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F105" s="2">
         <v>1</v>
@@ -2567,7 +2567,7 @@
         <v>21</v>
       </c>
       <c r="B106" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C106">
         <v>2016</v>
@@ -2576,7 +2576,7 @@
         <v>2</v>
       </c>
       <c r="E106" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F106" s="2">
         <v>1</v>
@@ -2587,7 +2587,7 @@
         <v>21</v>
       </c>
       <c r="B107" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C107">
         <v>2017</v>
@@ -2596,7 +2596,7 @@
         <v>1</v>
       </c>
       <c r="E107" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F107" s="2">
         <v>1</v>
@@ -2607,7 +2607,7 @@
         <v>21</v>
       </c>
       <c r="B108" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C108">
         <v>2017</v>
@@ -2616,7 +2616,7 @@
         <v>2</v>
       </c>
       <c r="E108" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F108" s="2">
         <v>1</v>
@@ -2627,7 +2627,7 @@
         <v>21</v>
       </c>
       <c r="B109" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C109">
         <v>2018</v>
@@ -2636,7 +2636,7 @@
         <v>1</v>
       </c>
       <c r="E109" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F109" s="2">
         <v>1</v>
@@ -2647,7 +2647,7 @@
         <v>21</v>
       </c>
       <c r="B110" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C110">
         <v>2018</v>
@@ -2656,7 +2656,7 @@
         <v>2</v>
       </c>
       <c r="E110" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F110" s="2">
         <v>1</v>
@@ -2667,7 +2667,7 @@
         <v>21</v>
       </c>
       <c r="B111" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C111">
         <v>2019</v>
@@ -2676,7 +2676,7 @@
         <v>1</v>
       </c>
       <c r="E111" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F111" s="2">
         <v>1</v>
@@ -2687,7 +2687,7 @@
         <v>21</v>
       </c>
       <c r="B112" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C112">
         <v>2019</v>
@@ -2696,7 +2696,7 @@
         <v>2</v>
       </c>
       <c r="E112" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F112" s="2">
         <v>1</v>
@@ -2707,7 +2707,7 @@
         <v>21</v>
       </c>
       <c r="B113" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C113">
         <v>2020</v>
@@ -2716,7 +2716,7 @@
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F113" s="2">
         <v>1</v>
@@ -2727,7 +2727,7 @@
         <v>21</v>
       </c>
       <c r="B114" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C114">
         <v>2020</v>
@@ -2736,7 +2736,7 @@
         <v>2</v>
       </c>
       <c r="E114" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F114" s="2">
         <v>1</v>
@@ -2747,7 +2747,7 @@
         <v>21</v>
       </c>
       <c r="B115" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C115">
         <v>2011</v>
@@ -2756,7 +2756,7 @@
         <v>1</v>
       </c>
       <c r="E115" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F115" s="2">
         <v>6</v>
@@ -2767,7 +2767,7 @@
         <v>21</v>
       </c>
       <c r="B116" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C116">
         <v>2011</v>
@@ -2776,7 +2776,7 @@
         <v>2</v>
       </c>
       <c r="E116" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F116" s="2">
         <v>6</v>
@@ -2787,7 +2787,7 @@
         <v>21</v>
       </c>
       <c r="B117" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C117">
         <v>2012</v>
@@ -2796,7 +2796,7 @@
         <v>1</v>
       </c>
       <c r="E117" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F117" s="2">
         <v>6</v>
@@ -2807,7 +2807,7 @@
         <v>21</v>
       </c>
       <c r="B118" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C118">
         <v>2012</v>
@@ -2816,7 +2816,7 @@
         <v>2</v>
       </c>
       <c r="E118" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F118" s="2">
         <v>6</v>
@@ -2827,7 +2827,7 @@
         <v>21</v>
       </c>
       <c r="B119" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C119">
         <v>2013</v>
@@ -2836,7 +2836,7 @@
         <v>1</v>
       </c>
       <c r="E119" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F119" s="2">
         <v>6</v>
@@ -2847,7 +2847,7 @@
         <v>21</v>
       </c>
       <c r="B120" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C120">
         <v>2013</v>
@@ -2856,7 +2856,7 @@
         <v>2</v>
       </c>
       <c r="E120" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F120" s="2">
         <v>6</v>
@@ -2867,7 +2867,7 @@
         <v>21</v>
       </c>
       <c r="B121" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C121">
         <v>2014</v>
@@ -2876,7 +2876,7 @@
         <v>1</v>
       </c>
       <c r="E121" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F121" s="2">
         <v>6</v>
@@ -2887,7 +2887,7 @@
         <v>21</v>
       </c>
       <c r="B122" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C122">
         <v>2014</v>
@@ -2896,7 +2896,7 @@
         <v>2</v>
       </c>
       <c r="E122" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F122" s="2">
         <v>6</v>
@@ -2907,7 +2907,7 @@
         <v>21</v>
       </c>
       <c r="B123" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C123">
         <v>2015</v>
@@ -2916,7 +2916,7 @@
         <v>1</v>
       </c>
       <c r="E123" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F123" s="2">
         <v>6</v>
@@ -2927,7 +2927,7 @@
         <v>21</v>
       </c>
       <c r="B124" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C124">
         <v>2015</v>
@@ -2936,7 +2936,7 @@
         <v>2</v>
       </c>
       <c r="E124" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F124" s="2">
         <v>6</v>
@@ -2947,7 +2947,7 @@
         <v>21</v>
       </c>
       <c r="B125" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C125">
         <v>2016</v>
@@ -2956,7 +2956,7 @@
         <v>1</v>
       </c>
       <c r="E125" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F125" s="2">
         <v>6</v>
@@ -2967,7 +2967,7 @@
         <v>21</v>
       </c>
       <c r="B126" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C126">
         <v>2016</v>
@@ -2976,7 +2976,7 @@
         <v>2</v>
       </c>
       <c r="E126" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F126" s="2">
         <v>6</v>
@@ -2987,7 +2987,7 @@
         <v>21</v>
       </c>
       <c r="B127" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C127">
         <v>2017</v>
@@ -2996,7 +2996,7 @@
         <v>1</v>
       </c>
       <c r="E127" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F127" s="2">
         <v>6</v>
@@ -3007,7 +3007,7 @@
         <v>21</v>
       </c>
       <c r="B128" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C128">
         <v>2017</v>
@@ -3016,7 +3016,7 @@
         <v>2</v>
       </c>
       <c r="E128" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F128" s="2">
         <v>6</v>
@@ -3027,7 +3027,7 @@
         <v>21</v>
       </c>
       <c r="B129" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C129">
         <v>2018</v>
@@ -3036,7 +3036,7 @@
         <v>1</v>
       </c>
       <c r="E129" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F129" s="2">
         <v>6</v>
@@ -3047,7 +3047,7 @@
         <v>21</v>
       </c>
       <c r="B130" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C130">
         <v>2018</v>
@@ -3056,7 +3056,7 @@
         <v>2</v>
       </c>
       <c r="E130" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F130" s="2">
         <v>6</v>
@@ -3067,7 +3067,7 @@
         <v>21</v>
       </c>
       <c r="B131" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C131">
         <v>2019</v>
@@ -3076,7 +3076,7 @@
         <v>1</v>
       </c>
       <c r="E131" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F131" s="2">
         <v>6</v>
@@ -3087,7 +3087,7 @@
         <v>21</v>
       </c>
       <c r="B132" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C132">
         <v>2019</v>
@@ -3096,7 +3096,7 @@
         <v>2</v>
       </c>
       <c r="E132" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F132" s="2">
         <v>6</v>
@@ -3107,7 +3107,7 @@
         <v>21</v>
       </c>
       <c r="B133" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C133">
         <v>2020</v>
@@ -3116,7 +3116,7 @@
         <v>1</v>
       </c>
       <c r="E133" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F133" s="2">
         <v>6</v>
@@ -3127,7 +3127,7 @@
         <v>21</v>
       </c>
       <c r="B134" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C134">
         <v>2020</v>
@@ -3136,7 +3136,7 @@
         <v>2</v>
       </c>
       <c r="E134" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F134" s="2">
         <v>6</v>
@@ -3147,7 +3147,7 @@
         <v>21</v>
       </c>
       <c r="B135" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C135">
         <v>2011</v>
@@ -3156,7 +3156,7 @@
         <v>1</v>
       </c>
       <c r="E135" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F135" s="2">
         <v>31</v>
@@ -3167,7 +3167,7 @@
         <v>21</v>
       </c>
       <c r="B136" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C136">
         <v>2011</v>
@@ -3176,7 +3176,7 @@
         <v>2</v>
       </c>
       <c r="E136" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F136" s="2">
         <v>33</v>
@@ -3187,7 +3187,7 @@
         <v>21</v>
       </c>
       <c r="B137" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C137">
         <v>2012</v>
@@ -3196,7 +3196,7 @@
         <v>1</v>
       </c>
       <c r="E137" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F137" s="2">
         <v>30</v>
@@ -3207,7 +3207,7 @@
         <v>21</v>
       </c>
       <c r="B138" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C138">
         <v>2012</v>
@@ -3216,7 +3216,7 @@
         <v>2</v>
       </c>
       <c r="E138" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F138" s="2">
         <v>35</v>
@@ -3227,7 +3227,7 @@
         <v>21</v>
       </c>
       <c r="B139" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C139">
         <v>2013</v>
@@ -3236,7 +3236,7 @@
         <v>1</v>
       </c>
       <c r="E139" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F139" s="2">
         <v>36</v>
@@ -3247,7 +3247,7 @@
         <v>21</v>
       </c>
       <c r="B140" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C140">
         <v>2013</v>
@@ -3256,7 +3256,7 @@
         <v>2</v>
       </c>
       <c r="E140" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F140" s="2">
         <v>37</v>
@@ -3267,7 +3267,7 @@
         <v>21</v>
       </c>
       <c r="B141" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C141">
         <v>2014</v>
@@ -3276,7 +3276,7 @@
         <v>1</v>
       </c>
       <c r="E141" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F141" s="2">
         <v>33</v>
@@ -3287,7 +3287,7 @@
         <v>21</v>
       </c>
       <c r="B142" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C142">
         <v>2014</v>
@@ -3296,7 +3296,7 @@
         <v>2</v>
       </c>
       <c r="E142" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F142" s="2">
         <v>37</v>
@@ -3307,7 +3307,7 @@
         <v>21</v>
       </c>
       <c r="B143" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C143">
         <v>2015</v>
@@ -3316,7 +3316,7 @@
         <v>1</v>
       </c>
       <c r="E143" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F143" s="2">
         <v>38</v>
@@ -3327,7 +3327,7 @@
         <v>21</v>
       </c>
       <c r="B144" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C144">
         <v>2015</v>
@@ -3336,7 +3336,7 @@
         <v>2</v>
       </c>
       <c r="E144" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F144" s="2">
         <v>40</v>
@@ -3347,7 +3347,7 @@
         <v>21</v>
       </c>
       <c r="B145" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C145">
         <v>2016</v>
@@ -3356,7 +3356,7 @@
         <v>1</v>
       </c>
       <c r="E145" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F145" s="2">
         <v>38</v>
@@ -3367,7 +3367,7 @@
         <v>21</v>
       </c>
       <c r="B146" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C146">
         <v>2016</v>
@@ -3376,7 +3376,7 @@
         <v>2</v>
       </c>
       <c r="E146" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F146" s="2">
         <v>40</v>
@@ -3387,7 +3387,7 @@
         <v>21</v>
       </c>
       <c r="B147" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C147">
         <v>2017</v>
@@ -3396,7 +3396,7 @@
         <v>1</v>
       </c>
       <c r="E147" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F147" s="2">
         <v>45</v>
@@ -3407,7 +3407,7 @@
         <v>21</v>
       </c>
       <c r="B148" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C148">
         <v>2017</v>
@@ -3416,7 +3416,7 @@
         <v>2</v>
       </c>
       <c r="E148" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F148" s="2">
         <v>45</v>
@@ -3427,7 +3427,7 @@
         <v>21</v>
       </c>
       <c r="B149" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C149">
         <v>2018</v>
@@ -3436,7 +3436,7 @@
         <v>1</v>
       </c>
       <c r="E149" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F149" s="2">
         <v>43</v>
@@ -3447,7 +3447,7 @@
         <v>21</v>
       </c>
       <c r="B150" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C150">
         <v>2018</v>
@@ -3456,7 +3456,7 @@
         <v>2</v>
       </c>
       <c r="E150" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F150" s="2">
         <v>40</v>
@@ -3467,7 +3467,7 @@
         <v>21</v>
       </c>
       <c r="B151" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C151">
         <v>2019</v>
@@ -3476,7 +3476,7 @@
         <v>1</v>
       </c>
       <c r="E151" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F151" s="2">
         <v>43</v>
@@ -3487,7 +3487,7 @@
         <v>21</v>
       </c>
       <c r="B152" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C152">
         <v>2019</v>
@@ -3496,7 +3496,7 @@
         <v>2</v>
       </c>
       <c r="E152" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F152" s="2">
         <v>42</v>
@@ -3507,7 +3507,7 @@
         <v>21</v>
       </c>
       <c r="B153" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C153">
         <v>2020</v>
@@ -3516,7 +3516,7 @@
         <v>1</v>
       </c>
       <c r="E153" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F153" s="2">
         <v>38</v>
@@ -3527,7 +3527,7 @@
         <v>21</v>
       </c>
       <c r="B154" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C154">
         <v>2020</v>
@@ -3536,7 +3536,7 @@
         <v>2</v>
       </c>
       <c r="E154" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F154" s="2">
         <v>42</v>

</xml_diff>